<commit_message>
Initial commit for quick selection java exercise.
</commit_message>
<xml_diff>
--- a/TC&SC.xlsx
+++ b/TC&SC.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/annzhou/data-structures-n-algorithms/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A43807F6-5F56-0F44-A996-8FAE38E2002F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F7328A3-4212-644C-9F16-436C88BE225F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="31920" yWindow="1540" windowWidth="17180" windowHeight="14660" xr2:uid="{8469AE36-E52C-BD4A-8888-A59A105D389E}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" xr2:uid="{8469AE36-E52C-BD4A-8888-A59A105D389E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="38">
   <si>
     <t>Algorithms</t>
   </si>
@@ -139,10 +139,6 @@
     <t>Binary Tree - getHeight</t>
   </si>
   <si>
-    <t>SC-Average
-O(height)</t>
-  </si>
-  <si>
     <t>blanaced or ~ linkedList</t>
   </si>
   <si>
@@ -150,6 +146,18 @@
   </si>
   <si>
     <t>Binary Tree - isBalanced</t>
+  </si>
+  <si>
+    <t>SC-AC</t>
+  </si>
+  <si>
+    <t>Time for each node</t>
+  </si>
+  <si>
+    <t>O(height), 粉色path的深度</t>
+  </si>
+  <si>
+    <t>Binary Tree - isSymmetric</t>
   </si>
 </sst>
 </file>
@@ -198,7 +206,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -208,7 +216,13 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -524,13 +538,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{53B6A48E-D328-B942-B4CC-F48B12BEF7EE}">
-  <dimension ref="A1:F15"/>
+  <dimension ref="A1:F17"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B18" sqref="B18"/>
+      <selection pane="bottomRight" activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="25.83203125" defaultRowHeight="16"/>
@@ -538,99 +552,98 @@
     <col min="1" max="1" width="26" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="24.33203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10.83203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="6.83203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.83203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="6.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.33203125" customWidth="1"/>
+    <col min="5" max="5" width="10.83203125" customWidth="1"/>
+    <col min="6" max="6" width="14" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="1" customFormat="1" ht="34">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:6" s="4" customFormat="1" ht="17">
+      <c r="C1" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="E1" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6">
-      <c r="A2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" t="s">
-        <v>2</v>
-      </c>
-      <c r="E2" t="s">
-        <v>6</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>5</v>
-      </c>
+      <c r="C2" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="D2" s="6"/>
+      <c r="E2" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="F2" s="6"/>
     </row>
     <row r="3" spans="1:6">
       <c r="A3" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="C3" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="E3" t="s">
-        <v>11</v>
+        <v>6</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:6">
       <c r="A4" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="B4" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="C4" t="s">
         <v>8</v>
       </c>
-      <c r="D4" t="s">
-        <v>2</v>
-      </c>
       <c r="E4" t="s">
-        <v>10</v>
-      </c>
-      <c r="F4" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="5" spans="1:6">
       <c r="A5" t="s">
-        <v>17</v>
+        <v>12</v>
+      </c>
+      <c r="B5" t="s">
+        <v>16</v>
       </c>
       <c r="C5" t="s">
-        <v>11</v>
+        <v>8</v>
+      </c>
+      <c r="D5" t="s">
+        <v>2</v>
       </c>
       <c r="E5" t="s">
-        <v>6</v>
+        <v>10</v>
+      </c>
+      <c r="F5" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="6" spans="1:6">
       <c r="A6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C6" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E6" t="s">
         <v>6</v>
@@ -638,96 +651,90 @@
     </row>
     <row r="7" spans="1:6">
       <c r="A7" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C7" t="s">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="E7" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:6" s="2" customFormat="1" ht="68">
-      <c r="A8" s="2" t="s">
+    <row r="8" spans="1:6">
+      <c r="A8" t="s">
+        <v>19</v>
+      </c>
+      <c r="C8" t="s">
+        <v>20</v>
+      </c>
+      <c r="E8" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" s="2" customFormat="1" ht="68">
+      <c r="A9" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="B8" s="3" t="s">
+      <c r="B9" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="C8" s="2" t="s">
+      <c r="C9" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="E8" s="2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6">
-      <c r="A9" t="s">
-        <v>24</v>
-      </c>
-      <c r="B9" t="s">
-        <v>26</v>
-      </c>
-      <c r="C9" t="s">
-        <v>25</v>
-      </c>
-      <c r="E9" t="s">
-        <v>25</v>
+      <c r="E9" s="2" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="10" spans="1:6">
       <c r="A10" t="s">
-        <v>27</v>
+        <v>24</v>
+      </c>
+      <c r="B10" t="s">
+        <v>26</v>
       </c>
       <c r="C10" t="s">
-        <v>11</v>
+        <v>25</v>
       </c>
       <c r="E10" t="s">
-        <v>6</v>
+        <v>25</v>
       </c>
     </row>
     <row r="11" spans="1:6">
       <c r="A11" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C11" t="s">
         <v>11</v>
+      </c>
+      <c r="E11" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="12" spans="1:6">
       <c r="A12" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C12" t="s">
-        <v>11</v>
-      </c>
-      <c r="E12" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="13" spans="1:6">
       <c r="A13" t="s">
-        <v>30</v>
-      </c>
-      <c r="B13" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="C13" t="s">
         <v>11</v>
       </c>
       <c r="E13" t="s">
-        <v>10</v>
-      </c>
-      <c r="F13" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="14" spans="1:6">
       <c r="A14" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="B14" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C14" t="s">
         <v>11</v>
@@ -741,16 +748,42 @@
     </row>
     <row r="15" spans="1:6">
       <c r="A15" t="s">
-        <v>34</v>
+        <v>32</v>
+      </c>
+      <c r="B15" t="s">
+        <v>31</v>
       </c>
       <c r="C15" t="s">
+        <v>11</v>
+      </c>
+      <c r="E15" t="s">
+        <v>10</v>
+      </c>
+      <c r="F15" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6">
+      <c r="A16" t="s">
+        <v>33</v>
+      </c>
+      <c r="C16" t="s">
         <v>8</v>
       </c>
-      <c r="E15" t="s">
-        <v>11</v>
+      <c r="E16" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1">
+      <c r="A17" t="s">
+        <v>37</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="E2:F2"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Initial commit for PreorderTraversalOfBinaryTree-iterative.java
</commit_message>
<xml_diff>
--- a/TC&SC.xlsx
+++ b/TC&SC.xlsx
@@ -8,13 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/annzhou/data-structures-n-algorithms/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F7328A3-4212-644C-9F16-436C88BE225F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4A6215A-EF35-FD46-B87D-C34A462E5031}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" xr2:uid="{8469AE36-E52C-BD4A-8888-A59A105D389E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$G$19</definedName>
+  </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -33,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="50">
   <si>
     <t>Algorithms</t>
   </si>
@@ -93,15 +96,9 @@
     <t>SC-WC</t>
   </si>
   <si>
-    <t>选pivot</t>
-  </si>
-  <si>
     <t>Rainbow Sort</t>
   </si>
   <si>
-    <t>Binary Search</t>
-  </si>
-  <si>
     <t>Binary Search Matrix</t>
   </si>
   <si>
@@ -111,16 +108,6 @@
     <t>O(2^n)</t>
   </si>
   <si>
-    <t>TC: sum of the time of each node
-SC: tree height</t>
-  </si>
-  <si>
-    <t>Recursion - fib() - bad</t>
-  </si>
-  <si>
-    <t>Recursion - Power</t>
-  </si>
-  <si>
     <t>O(b)</t>
   </si>
   <si>
@@ -139,9 +126,6 @@
     <t>Binary Tree - getHeight</t>
   </si>
   <si>
-    <t>blanaced or ~ linkedList</t>
-  </si>
-  <si>
     <t>Binary Tree - countNode</t>
   </si>
   <si>
@@ -151,23 +135,141 @@
     <t>SC-AC</t>
   </si>
   <si>
-    <t>Time for each node</t>
-  </si>
-  <si>
-    <t>O(height), 粉色path的深度</t>
+    <t>O(height)</t>
   </si>
   <si>
     <t>Binary Tree - isSymmetric</t>
+  </si>
+  <si>
+    <t>O(n/2) = O(n)</t>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>O(log(b))</t>
+  </si>
+  <si>
+    <t>fib() - recursive</t>
+  </si>
+  <si>
+    <t>fib() - iterative</t>
+  </si>
+  <si>
+    <t>Bad; # of nodes = 2^0 + 2^1 + ... + 2^(n-1) = 2^n</t>
+  </si>
+  <si>
+    <t>WC: 每次pivot都选到最值</t>
+  </si>
+  <si>
+    <t>power - recursive - 2 个 RC</t>
+  </si>
+  <si>
+    <t>Review</t>
+  </si>
+  <si>
+    <t>Sum of time spent for each node</t>
+  </si>
+  <si>
+    <t>blanaced vs ~linkedList</t>
+  </si>
+  <si>
+    <t>Recursive: O(height), 粉色path的深度</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">TC: How many times do we need to divide 2 till there is only 1 element left?  </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t>n / 2^k =&gt; k = log(n) 指数衰减</t>
+    </r>
+  </si>
+  <si>
+    <t>b / 2^L = 1 =&gt; L = log(b) 指数衰减</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Binary Search
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t xml:space="preserve">mid = left + (right - left) </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t>/ 2</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">power - recursive - 1 个 RC </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t>half = power(a, b</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t>/2</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t>)</t>
+    </r>
+  </si>
+  <si>
+    <t>mn = number of elements in the 2D array</t>
+  </si>
+  <si>
+    <t>每次return都是两个RC一起，所以n/2</t>
+  </si>
+  <si>
+    <t>TC: 调用了n 次recursive function</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3">
+  <fonts count="6">
     <font>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -185,16 +287,65 @@
       <color rgb="FFFF0000"/>
       <name val="Calibri (Body)"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFFF85FF"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri (Body)"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -202,27 +353,81 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -230,6 +435,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFFF85FF"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -538,251 +748,339 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{53B6A48E-D328-B942-B4CC-F48B12BEF7EE}">
-  <dimension ref="A1:F17"/>
+  <dimension ref="A1:G19"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C17" sqref="C17"/>
+      <selection pane="bottomRight" activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="25.83203125" defaultRowHeight="16"/>
   <cols>
-    <col min="1" max="1" width="26" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="24.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.83203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.33203125" customWidth="1"/>
-    <col min="5" max="5" width="10.83203125" customWidth="1"/>
-    <col min="6" max="6" width="14" customWidth="1"/>
+    <col min="1" max="1" width="7.33203125" style="10" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="26" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="34.5" style="1" customWidth="1"/>
+    <col min="4" max="4" width="12.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.83203125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="10.83203125" style="1" customWidth="1"/>
+    <col min="7" max="7" width="14" style="1" customWidth="1"/>
+    <col min="8" max="16384" width="25.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="4" customFormat="1" ht="17">
-      <c r="C1" s="4" t="s">
+    <row r="1" spans="1:7" s="12" customFormat="1" ht="17">
+      <c r="A1" s="4"/>
+      <c r="B1" s="4"/>
+      <c r="C1" s="4"/>
+      <c r="D1" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="E1" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="F1" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" s="10" customFormat="1" ht="34" customHeight="1">
+      <c r="A2" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="E2" s="13"/>
+      <c r="F2" s="14" t="s">
+        <v>42</v>
+      </c>
+      <c r="G2" s="14"/>
+    </row>
+    <row r="3" spans="1:7" ht="51">
+      <c r="A3" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="34">
+      <c r="A4" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="17">
+      <c r="A5" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="34">
+      <c r="A6" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="B6" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="F1" s="4" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6">
-      <c r="A2" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C2" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="D2" s="6"/>
-      <c r="E2" s="6" t="s">
+      <c r="C6" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="F2" s="6"/>
-    </row>
-    <row r="3" spans="1:6">
-      <c r="A3" t="s">
+      <c r="D6" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="17">
+      <c r="A7" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="34">
+      <c r="A8" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="17">
+      <c r="A9" s="7"/>
+      <c r="B9" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C9" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D9" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F9" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="F3" s="1" t="s">
+      <c r="G9" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
-      <c r="A4" t="s">
+    <row r="10" spans="1:7" ht="17">
+      <c r="A10" s="7"/>
+      <c r="B10" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C10" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D10" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E4" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6">
-      <c r="A5" t="s">
+      <c r="F10" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="17">
+      <c r="A11" s="7"/>
+      <c r="B11" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B5" t="s">
+      <c r="C11" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="17">
+      <c r="A12" s="7"/>
+      <c r="B12" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C5" t="s">
+      <c r="D12" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="17">
+      <c r="A13" s="8"/>
+      <c r="B13" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="17">
+      <c r="A14" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F14" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="17">
+      <c r="A15" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" ht="17">
+      <c r="A16" s="9"/>
+      <c r="B16" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G16" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" ht="17">
+      <c r="A17" s="9"/>
+      <c r="B17" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G17" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" ht="17">
+      <c r="A18" s="9"/>
+      <c r="B18" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D18" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D5" t="s">
-        <v>2</v>
-      </c>
-      <c r="E5" t="s">
-        <v>10</v>
-      </c>
-      <c r="F5" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6">
-      <c r="A6" t="s">
-        <v>17</v>
-      </c>
-      <c r="C6" t="s">
-        <v>11</v>
-      </c>
-      <c r="E6" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6">
-      <c r="A7" t="s">
-        <v>18</v>
-      </c>
-      <c r="C7" t="s">
-        <v>10</v>
-      </c>
-      <c r="E7" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6">
-      <c r="A8" t="s">
-        <v>19</v>
-      </c>
-      <c r="C8" t="s">
-        <v>20</v>
-      </c>
-      <c r="E8" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" s="2" customFormat="1" ht="68">
-      <c r="A9" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="B9" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="E9" s="2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6">
-      <c r="A10" t="s">
-        <v>24</v>
-      </c>
-      <c r="B10" t="s">
-        <v>26</v>
-      </c>
-      <c r="C10" t="s">
-        <v>25</v>
-      </c>
-      <c r="E10" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6">
-      <c r="A11" t="s">
-        <v>27</v>
-      </c>
-      <c r="C11" t="s">
-        <v>11</v>
-      </c>
-      <c r="E11" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6">
-      <c r="A12" t="s">
-        <v>28</v>
-      </c>
-      <c r="C12" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6">
-      <c r="A13" t="s">
+      <c r="F18" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" ht="17">
+      <c r="A19" s="9"/>
+      <c r="B19" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="F19" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="C13" t="s">
-        <v>11</v>
-      </c>
-      <c r="E13" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6">
-      <c r="A14" t="s">
-        <v>30</v>
-      </c>
-      <c r="B14" t="s">
-        <v>31</v>
-      </c>
-      <c r="C14" t="s">
-        <v>11</v>
-      </c>
-      <c r="E14" t="s">
-        <v>10</v>
-      </c>
-      <c r="F14" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6">
-      <c r="A15" t="s">
-        <v>32</v>
-      </c>
-      <c r="B15" t="s">
-        <v>31</v>
-      </c>
-      <c r="C15" t="s">
-        <v>11</v>
-      </c>
-      <c r="E15" t="s">
-        <v>10</v>
-      </c>
-      <c r="F15" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6">
-      <c r="A16" t="s">
-        <v>33</v>
-      </c>
-      <c r="C16" t="s">
-        <v>8</v>
-      </c>
-      <c r="E16" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1">
-      <c r="A17" t="s">
-        <v>37</v>
-      </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:G19" xr:uid="{DDC5B641-DB79-EA4E-8C7D-66A8211CB31E}"/>
   <mergeCells count="2">
-    <mergeCell ref="C2:D2"/>
-    <mergeCell ref="E2:F2"/>
+    <mergeCell ref="D2:E2"/>
+    <mergeCell ref="F2:G2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Initial commit for check if a binary tree is completed java file
</commit_message>
<xml_diff>
--- a/TC&SC.xlsx
+++ b/TC&SC.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/annzhou/data-structures-n-algorithms/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4A6215A-EF35-FD46-B87D-C34A462E5031}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61DAC5BD-3661-0F47-A847-3CB2EAE0C447}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" xr2:uid="{8469AE36-E52C-BD4A-8888-A59A105D389E}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="51">
   <si>
     <t>Algorithms</t>
   </si>
@@ -253,6 +253,10 @@
   </si>
   <si>
     <t>TC: 调用了n 次recursive function</t>
+  </si>
+  <si>
+    <t>每个node都要调用一次getHeight(node) recursive function, 总共有n个node，所以TC = O(n)
+SC = O(height) - blanaced vs ~linkedList</t>
   </si>
 </sst>
 </file>
@@ -754,14 +758,14 @@
       <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E16" sqref="E16"/>
+      <selection pane="bottomRight" activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="25.83203125" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="7.33203125" style="10" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="26" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="34.5" style="1" customWidth="1"/>
+    <col min="3" max="3" width="36.1640625" style="1" customWidth="1"/>
     <col min="4" max="4" width="12.33203125" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="7.83203125" style="1" customWidth="1"/>
     <col min="6" max="6" width="10.83203125" style="1" customWidth="1"/>
@@ -1013,13 +1017,15 @@
         <v>11</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="17">
-      <c r="A16" s="9"/>
+    <row r="16" spans="1:7" ht="68">
+      <c r="A16" s="9" t="s">
+        <v>32</v>
+      </c>
       <c r="B16" s="1" t="s">
         <v>25</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>41</v>
+        <v>50</v>
       </c>
       <c r="D16" s="1" t="s">
         <v>11</v>

</xml_diff>